<commit_message>
metrics and summary of training
</commit_message>
<xml_diff>
--- a/03_devnagari_classification/summary.xlsx
+++ b/03_devnagari_classification/summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
   <si>
     <t xml:space="preserve">Devanagari Handwritten Iteration Details</t>
   </si>
@@ -49,7 +49,7 @@
     <t xml:space="preserve">Datasets</t>
   </si>
   <si>
-    <t xml:space="preserve">Final Accuracy</t>
+    <t xml:space="preserve">Final Accuracy(%)</t>
   </si>
   <si>
     <t xml:space="preserve">Remarks</t>
@@ -64,7 +64,7 @@
     <t xml:space="preserve">Test</t>
   </si>
   <si>
-    <t xml:space="preserve">v1.1</t>
+    <t xml:space="preserve">V1.0</t>
   </si>
   <si>
     <t xml:space="preserve">ResNet50</t>
@@ -74,6 +74,21 @@
   </si>
   <si>
     <t xml:space="preserve">Cross Entropy </t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Learning rate is decreased so is accuracy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Increased learning rate which also increased accuracy slightly.</t>
   </si>
 </sst>
 </file>
@@ -89,6 +104,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -110,6 +126,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -154,17 +171,13 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -192,23 +205,26 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:M6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="10.05"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.93"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="12.68"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="6.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.48"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -227,6 +243,7 @@
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
       <c r="M1" s="1"/>
+      <c r="N1" s="1"/>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
@@ -259,7 +276,8 @@
         <v>9</v>
       </c>
       <c r="L2" s="1"/>
-      <c r="M2" s="2" t="s">
+      <c r="M2" s="1"/>
+      <c r="N2" s="2" t="s">
         <v>10</v>
       </c>
     </row>
@@ -271,20 +289,23 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
-      <c r="H3" s="3" t="s">
+      <c r="H3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="I3" s="3" t="s">
+      <c r="I3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="3" t="s">
+      <c r="J3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="K3" s="3" t="s">
+      <c r="K3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="L3" s="2" t="s">
         <v>12</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -306,31 +327,139 @@
       <c r="F4" s="0" t="s">
         <v>17</v>
       </c>
-      <c r="G4" s="4" t="n">
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E5" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="n">
         <v>1.5E-005</v>
       </c>
-      <c r="H4" s="0" t="n">
+      <c r="H5" s="0" t="n">
         <v>58647</v>
       </c>
-      <c r="I4" s="0" t="n">
-        <v>19548</v>
-      </c>
-      <c r="J4" s="0" t="n">
-        <v>27600</v>
-      </c>
-      <c r="K4" s="0" t="n">
+      <c r="I5" s="0" t="n">
+        <v>19550</v>
+      </c>
+      <c r="J5" s="0" t="n">
+        <v>27599</v>
+      </c>
+      <c r="K5" s="0" t="n">
         <v>99.88</v>
       </c>
-      <c r="L4" s="0" t="n">
+      <c r="L5" s="0" t="n">
         <v>98.93</v>
       </c>
+      <c r="M5" s="0" t="n">
+        <v>98.93</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="G6" s="4"/>
+      <c r="A6" s="0" t="s">
+        <v>19</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E6" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="0" t="n">
+        <v>7.5E-006</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>58647</v>
+      </c>
+      <c r="I6" s="0" t="n">
+        <v>19550</v>
+      </c>
+      <c r="J6" s="0" t="n">
+        <v>27599</v>
+      </c>
+      <c r="K6" s="0" t="n">
+        <v>98.64</v>
+      </c>
+      <c r="L6" s="0" t="n">
+        <v>97.6</v>
+      </c>
+      <c r="M6" s="0" t="n">
+        <v>97.72</v>
+      </c>
+      <c r="N6" s="0" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3" t="n">
+        <v>1.55E-005</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>58647</v>
+      </c>
+      <c r="I7" s="0" t="n">
+        <v>19550</v>
+      </c>
+      <c r="J7" s="0" t="n">
+        <v>27599</v>
+      </c>
+      <c r="K7" s="0" t="n">
+        <v>99.91</v>
+      </c>
+      <c r="L7" s="0" t="n">
+        <v>98.94</v>
+      </c>
+      <c r="M7" s="0" t="n">
+        <v>99.06</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>22</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
-    <mergeCell ref="A1:M1"/>
+    <mergeCell ref="A1:N1"/>
     <mergeCell ref="A2:A3"/>
     <mergeCell ref="B2:B3"/>
     <mergeCell ref="C2:C3"/>
@@ -339,7 +468,7 @@
     <mergeCell ref="F2:F3"/>
     <mergeCell ref="G2:G3"/>
     <mergeCell ref="H2:J2"/>
-    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="K2:M2"/>
   </mergeCells>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
updated summary of training
</commit_message>
<xml_diff>
--- a/03_devnagari_classification/summary.xlsx
+++ b/03_devnagari_classification/summary.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="26">
   <si>
     <t xml:space="preserve">Devanagari Handwritten Iteration Details</t>
   </si>
@@ -89,6 +89,15 @@
   </si>
   <si>
     <t xml:space="preserve">Increased learning rate which also increased accuracy slightly.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1.3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Took v1.3 classifier, retrained it decreasing the learning rate and result obtained is remarkable.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">V1.3.2</t>
   </si>
 </sst>
 </file>
@@ -205,13 +214,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N7"/>
+  <dimension ref="A1:N9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I16" activeCellId="0" sqref="I16"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="N19" activeCellId="0" sqref="N19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.1"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="9.35"/>
@@ -224,7 +233,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="10.19"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="6.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="50.48"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="77.43"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -455,6 +464,67 @@
       </c>
       <c r="N7" s="0" t="s">
         <v>22</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="n">
+        <v>1.25E-006</v>
+      </c>
+      <c r="K8" s="0" t="n">
+        <v>99.63</v>
+      </c>
+      <c r="L8" s="0" t="n">
+        <v>99.68</v>
+      </c>
+      <c r="N8" s="0" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" s="3" t="n">
+        <v>1.25E-006</v>
+      </c>
+      <c r="K9" s="0" t="n">
+        <v>99.7</v>
+      </c>
+      <c r="L9" s="0" t="n">
+        <v>99.72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>